<commit_message>
update design login, logut, change-password
</commit_message>
<xml_diff>
--- a/BD/FILE_LIST_MSG.xlsx
+++ b/BD/FILE_LIST_MSG.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\www\QLNV\QLNV_document\BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\quanlynhansu\QLNV_document\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D47EE2-4C67-4DA8-87F7-B127F86E9392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942D7923-C42A-4DD0-B9F2-24D4D95C223B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Your password and confirm password do not match.</t>
   </si>
   <si>
-    <t>The password field must be 12 or more character in length and including UPPER/lowercase and number</t>
-  </si>
-  <si>
     <t>MSG_008</t>
   </si>
   <si>
@@ -94,13 +91,29 @@
   </si>
   <si>
     <t>MSG_010</t>
+  </si>
+  <si>
+    <t>MSG_011</t>
+  </si>
+  <si>
+    <t>Are you sure you want to logout?</t>
+  </si>
+  <si>
+    <t>MSG_012</t>
+  </si>
+  <si>
+    <t>Sesion Expired
+Please login again.</t>
+  </si>
+  <si>
+    <t>Invalid password.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +125,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +193,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:E37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -559,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>17</v>
@@ -570,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>18</v>
@@ -581,21 +608,33 @@
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="7">
+        <v>12</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
@@ -708,6 +747,7 @@
       <c r="E37" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>